<commit_message>
3.19 2 easy 2 medium array
</commit_message>
<xml_diff>
--- a/leetcode.xlsx
+++ b/leetcode.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LeetCode-Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2070BC94-42DA-4BD2-A99B-C8F026CB487E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68187DF1-B50B-4184-97BE-11DB9F024ABD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1103" yWindow="1103" windowWidth="14400" windowHeight="7372" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="leetcode" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3149" uniqueCount="1257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3163" uniqueCount="1259">
   <si>
     <t>题号</t>
   </si>
@@ -3791,6 +3791,12 @@
   </si>
   <si>
     <t>binary search</t>
+  </si>
+  <si>
+    <t>dp</t>
+  </si>
+  <si>
+    <t>array dp</t>
   </si>
 </sst>
 </file>
@@ -4651,8 +4657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H619"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A326" workbookViewId="0">
-      <selection activeCell="I333" sqref="I333"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -4914,6 +4920,12 @@
       <c r="F12" t="s">
         <v>11</v>
       </c>
+      <c r="G12" t="s">
+        <v>1250</v>
+      </c>
+      <c r="H12" t="s">
+        <v>1252</v>
+      </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13">
@@ -5026,6 +5038,12 @@
       <c r="F17" t="s">
         <v>11</v>
       </c>
+      <c r="G17" t="s">
+        <v>1250</v>
+      </c>
+      <c r="H17" t="s">
+        <v>1252</v>
+      </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18">
@@ -5653,7 +5671,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:8">
       <c r="A49">
         <v>48</v>
       </c>
@@ -5673,7 +5691,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:8">
       <c r="A50">
         <v>49</v>
       </c>
@@ -5696,7 +5714,7 @@
         <v>1249</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:8">
       <c r="A51">
         <v>50</v>
       </c>
@@ -5716,7 +5734,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:8">
       <c r="A52">
         <v>51</v>
       </c>
@@ -5736,7 +5754,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:8">
       <c r="A53">
         <v>52</v>
       </c>
@@ -5756,7 +5774,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:8">
       <c r="A54">
         <v>53</v>
       </c>
@@ -5775,8 +5793,14 @@
       <c r="F54" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="55" spans="1:7">
+      <c r="G54" t="s">
+        <v>1249</v>
+      </c>
+      <c r="H54" t="s">
+        <v>1257</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
       <c r="A55">
         <v>54</v>
       </c>
@@ -5796,7 +5820,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:8">
       <c r="A56">
         <v>55</v>
       </c>
@@ -5816,7 +5840,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:8">
       <c r="A57">
         <v>56</v>
       </c>
@@ -5836,7 +5860,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:8">
       <c r="A58">
         <v>57</v>
       </c>
@@ -5856,7 +5880,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:8">
       <c r="A59">
         <v>58</v>
       </c>
@@ -5876,7 +5900,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:8">
       <c r="A60">
         <v>59</v>
       </c>
@@ -5896,7 +5920,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:8">
       <c r="A61">
         <v>60</v>
       </c>
@@ -5916,7 +5940,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:8">
       <c r="A62">
         <v>61</v>
       </c>
@@ -5936,7 +5960,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:8">
       <c r="A63">
         <v>62</v>
       </c>
@@ -5956,7 +5980,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:8">
       <c r="A64">
         <v>63</v>
       </c>
@@ -6127,6 +6151,12 @@
       <c r="F71" t="s">
         <v>11</v>
       </c>
+      <c r="G71" t="s">
+        <v>1254</v>
+      </c>
+      <c r="H71" t="s">
+        <v>1257</v>
+      </c>
     </row>
     <row r="72" spans="1:8">
       <c r="A72">
@@ -7108,6 +7138,12 @@
       <c r="F119" t="s">
         <v>11</v>
       </c>
+      <c r="G119" t="s">
+        <v>1249</v>
+      </c>
+      <c r="H119" t="s">
+        <v>1252</v>
+      </c>
     </row>
     <row r="120" spans="1:8">
       <c r="A120">
@@ -7128,6 +7164,12 @@
       <c r="F120" t="s">
         <v>11</v>
       </c>
+      <c r="G120" t="s">
+        <v>1249</v>
+      </c>
+      <c r="H120" t="s">
+        <v>1252</v>
+      </c>
     </row>
     <row r="121" spans="1:8">
       <c r="A121">
@@ -7172,7 +7214,7 @@
         <v>1254</v>
       </c>
       <c r="H122" t="s">
-        <v>1252</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="123" spans="1:8">
@@ -8279,7 +8321,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="177" spans="1:6">
+    <row r="177" spans="1:8">
       <c r="A177">
         <v>186</v>
       </c>
@@ -8299,7 +8341,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="178" spans="1:6">
+    <row r="178" spans="1:8">
       <c r="A178">
         <v>187</v>
       </c>
@@ -8319,7 +8361,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="179" spans="1:6">
+    <row r="179" spans="1:8">
       <c r="A179">
         <v>188</v>
       </c>
@@ -8339,7 +8381,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="180" spans="1:6">
+    <row r="180" spans="1:8">
       <c r="A180">
         <v>189</v>
       </c>
@@ -8359,7 +8401,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="181" spans="1:6">
+    <row r="181" spans="1:8">
       <c r="A181">
         <v>190</v>
       </c>
@@ -8379,7 +8421,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="182" spans="1:6">
+    <row r="182" spans="1:8">
       <c r="A182">
         <v>191</v>
       </c>
@@ -8399,7 +8441,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="183" spans="1:6">
+    <row r="183" spans="1:8">
       <c r="A183">
         <v>198</v>
       </c>
@@ -8418,8 +8460,14 @@
       <c r="F183" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="184" spans="1:6">
+      <c r="G183" t="s">
+        <v>1254</v>
+      </c>
+      <c r="H183" t="s">
+        <v>1257</v>
+      </c>
+    </row>
+    <row r="184" spans="1:8">
       <c r="A184">
         <v>199</v>
       </c>
@@ -8439,7 +8487,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="185" spans="1:6">
+    <row r="185" spans="1:8">
       <c r="A185">
         <v>200</v>
       </c>
@@ -8459,7 +8507,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="186" spans="1:6">
+    <row r="186" spans="1:8">
       <c r="A186">
         <v>201</v>
       </c>
@@ -8479,7 +8527,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="187" spans="1:6">
+    <row r="187" spans="1:8">
       <c r="A187">
         <v>202</v>
       </c>
@@ -8499,7 +8547,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="188" spans="1:6">
+    <row r="188" spans="1:8">
       <c r="A188">
         <v>203</v>
       </c>
@@ -8519,7 +8567,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="189" spans="1:6">
+    <row r="189" spans="1:8">
       <c r="A189">
         <v>204</v>
       </c>
@@ -8539,7 +8587,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="190" spans="1:6">
+    <row r="190" spans="1:8">
       <c r="A190">
         <v>205</v>
       </c>
@@ -8559,7 +8607,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="191" spans="1:6">
+    <row r="191" spans="1:8">
       <c r="A191">
         <v>206</v>
       </c>
@@ -8579,7 +8627,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="192" spans="1:6">
+    <row r="192" spans="1:8">
       <c r="A192">
         <v>207</v>
       </c>

</xml_diff>